<commit_message>
set 600km for MP supply chain relationship
</commit_message>
<xml_diff>
--- a/Data/coal_supply_chain_india.xlsx
+++ b/Data/coal_supply_chain_india.xlsx
@@ -74538,7 +74538,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D330"/>
+  <dimension ref="A1:D294"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -74576,7 +74576,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4483696409516553</v>
+        <v>0.2357085905558797</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -74592,7 +74592,7 @@
         <v>88</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7303945729119798</v>
+        <v>0.3071507711258369</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -74608,7 +74608,7 @@
         <v>141</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9585994352310032</v>
+        <v>0.5949770375462405</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -74624,7 +74624,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1555626074763143</v>
+        <v>0.4611166190745661</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -74640,7 +74640,7 @@
         <v>88</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5108083944368675</v>
+        <v>0.03558535783282513</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -74656,7 +74656,7 @@
         <v>141</v>
       </c>
       <c r="C7" t="n">
-        <v>0.691704948839069</v>
+        <v>0.1927174529293064</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -74672,7 +74672,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2119362682102967</v>
+        <v>0.08093572067535026</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -74688,7 +74688,7 @@
         <v>88</v>
       </c>
       <c r="C9" t="n">
-        <v>0.01596767981498137</v>
+        <v>0.6548469321202219</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -74704,7 +74704,7 @@
         <v>141</v>
       </c>
       <c r="C10" t="n">
-        <v>0.5088768803746553</v>
+        <v>0.3709720993196116</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -74720,7 +74720,7 @@
         <v>8</v>
       </c>
       <c r="C11" t="n">
-        <v>0.9616462476806465</v>
+        <v>0.1733477990962073</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -74736,7 +74736,7 @@
         <v>88</v>
       </c>
       <c r="C12" t="n">
-        <v>0.331399741827763</v>
+        <v>0.4566813884078065</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -74752,7 +74752,7 @@
         <v>141</v>
       </c>
       <c r="C13" t="n">
-        <v>0.4980429481944755</v>
+        <v>0.4139489534617852</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -74768,7 +74768,7 @@
         <v>142</v>
       </c>
       <c r="C14" t="n">
-        <v>0.5276186751016801</v>
+        <v>0.1865056148494725</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -74784,7 +74784,7 @@
         <v>157</v>
       </c>
       <c r="C15" t="n">
-        <v>0.3343809798454428</v>
+        <v>0.7130277662558818</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -74800,7 +74800,7 @@
         <v>48</v>
       </c>
       <c r="C16" t="n">
-        <v>0.5240031471691972</v>
+        <v>0.4175040146423721</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -74816,7 +74816,7 @@
         <v>110</v>
       </c>
       <c r="C17" t="n">
-        <v>0.966787329260317</v>
+        <v>0.8961302109534393</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -74832,7 +74832,7 @@
         <v>155</v>
       </c>
       <c r="C18" t="n">
-        <v>0.8622373333673145</v>
+        <v>0.8769401232080475</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -74848,7 +74848,7 @@
         <v>162</v>
       </c>
       <c r="C19" t="n">
-        <v>0.9050658311726921</v>
+        <v>0.6710906064209406</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -74864,7 +74864,7 @@
         <v>98</v>
       </c>
       <c r="C20" t="n">
-        <v>0.8751976317566956</v>
+        <v>0.1265159419541377</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -74880,7 +74880,7 @@
         <v>47</v>
       </c>
       <c r="C21" t="n">
-        <v>0.9756010517183591</v>
+        <v>0.265055828643352</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -74896,7 +74896,7 @@
         <v>47</v>
       </c>
       <c r="C22" t="n">
-        <v>0.7990807465004571</v>
+        <v>0.07316808510080219</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -74912,7 +74912,7 @@
         <v>140</v>
       </c>
       <c r="C23" t="n">
-        <v>0.9328501367506986</v>
+        <v>0.6283698966709994</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -74928,7 +74928,7 @@
         <v>143</v>
       </c>
       <c r="C24" t="n">
-        <v>0.9624041761907355</v>
+        <v>0.4233885409025245</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -74944,7 +74944,7 @@
         <v>142</v>
       </c>
       <c r="C25" t="n">
-        <v>0.9346632167051664</v>
+        <v>0.6771922415793922</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -74960,7 +74960,7 @@
         <v>143</v>
       </c>
       <c r="C26" t="n">
-        <v>0.5286405698426424</v>
+        <v>0.2770140461271174</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -74976,7 +74976,7 @@
         <v>157</v>
       </c>
       <c r="C27" t="n">
-        <v>0.8819989900200707</v>
+        <v>0.6003706975876609</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -74992,7 +74992,7 @@
         <v>162</v>
       </c>
       <c r="C28" t="n">
-        <v>0.7987167802462214</v>
+        <v>0.3267102498832313</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -75008,7 +75008,7 @@
         <v>48</v>
       </c>
       <c r="C29" t="n">
-        <v>0.963224835292768</v>
+        <v>0.9420287671034804</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -75024,7 +75024,7 @@
         <v>11</v>
       </c>
       <c r="C30" t="n">
-        <v>0.650027548027417</v>
+        <v>0.9272782809902209</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -75040,7 +75040,7 @@
         <v>104</v>
       </c>
       <c r="C31" t="n">
-        <v>0.7157943491419594</v>
+        <v>0.4466339942718587</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -75056,7 +75056,7 @@
         <v>117</v>
       </c>
       <c r="C32" t="n">
-        <v>0.01109679777954176</v>
+        <v>0.7901500336577097</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -75072,7 +75072,7 @@
         <v>82</v>
       </c>
       <c r="C33" t="n">
-        <v>0.7078013071569018</v>
+        <v>0.3880991421107765</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -75088,7 +75088,7 @@
         <v>59</v>
       </c>
       <c r="C34" t="n">
-        <v>0.1603982254673655</v>
+        <v>0.815179138945177</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -75104,7 +75104,7 @@
         <v>11</v>
       </c>
       <c r="C35" t="n">
-        <v>0.5825657411957949</v>
+        <v>0.5516232056537573</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -75120,7 +75120,7 @@
         <v>142</v>
       </c>
       <c r="C36" t="n">
-        <v>0.0665443718550357</v>
+        <v>0.8456367321148353</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -75136,7 +75136,7 @@
         <v>143</v>
       </c>
       <c r="C37" t="n">
-        <v>0.1698415457053043</v>
+        <v>0.8488759981875411</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -75152,7 +75152,7 @@
         <v>104</v>
       </c>
       <c r="C38" t="n">
-        <v>0.1363207913218161</v>
+        <v>0.7366160164720411</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -75168,7 +75168,7 @@
         <v>117</v>
       </c>
       <c r="C39" t="n">
-        <v>0.3327456862512913</v>
+        <v>0.5557634841139927</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -75184,7 +75184,7 @@
         <v>82</v>
       </c>
       <c r="C40" t="n">
-        <v>0.5999822155344869</v>
+        <v>0.008376443426887259</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -75200,7 +75200,7 @@
         <v>155</v>
       </c>
       <c r="C41" t="n">
-        <v>0.7810630487901981</v>
+        <v>0.7802589674794325</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -75216,7 +75216,7 @@
         <v>162</v>
       </c>
       <c r="C42" t="n">
-        <v>0.6533747500937435</v>
+        <v>0.007176614328941899</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -75232,7 +75232,7 @@
         <v>59</v>
       </c>
       <c r="C43" t="n">
-        <v>0.4652323446336829</v>
+        <v>0.3266150468406718</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -75248,7 +75248,7 @@
         <v>47</v>
       </c>
       <c r="C44" t="n">
-        <v>0.3429547614699273</v>
+        <v>0.1558254702291941</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -75264,7 +75264,7 @@
         <v>47</v>
       </c>
       <c r="C45" t="n">
-        <v>0.8129720780896845</v>
+        <v>0.5059547796860022</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -75280,7 +75280,7 @@
         <v>11</v>
       </c>
       <c r="C46" t="n">
-        <v>0.220088127661925</v>
+        <v>0.430585049661879</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -75296,7 +75296,7 @@
         <v>142</v>
       </c>
       <c r="C47" t="n">
-        <v>0.2339383000143442</v>
+        <v>0.5826332081925143</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -75312,7 +75312,7 @@
         <v>143</v>
       </c>
       <c r="C48" t="n">
-        <v>0.1174046516667554</v>
+        <v>0.1911251052793677</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -75328,7 +75328,7 @@
         <v>110</v>
       </c>
       <c r="C49" t="n">
-        <v>0.4323392035913245</v>
+        <v>0.8187236192383831</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -75344,7 +75344,7 @@
         <v>104</v>
       </c>
       <c r="C50" t="n">
-        <v>0.9694782605533691</v>
+        <v>0.1130975242494405</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -75360,7 +75360,7 @@
         <v>117</v>
       </c>
       <c r="C51" t="n">
-        <v>0.1700447548092213</v>
+        <v>0.7012149464137845</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -75376,7 +75376,7 @@
         <v>82</v>
       </c>
       <c r="C52" t="n">
-        <v>0.9119195140935095</v>
+        <v>0.2900984166880989</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -75392,7 +75392,7 @@
         <v>155</v>
       </c>
       <c r="C53" t="n">
-        <v>0.9823247527640828</v>
+        <v>0.5445499835540325</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -75408,7 +75408,7 @@
         <v>162</v>
       </c>
       <c r="C54" t="n">
-        <v>0.6041781440170962</v>
+        <v>0.9037489930253323</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -75424,7 +75424,7 @@
         <v>59</v>
       </c>
       <c r="C55" t="n">
-        <v>0.2967291683198606</v>
+        <v>0.876176974404837</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -75440,7 +75440,7 @@
         <v>47</v>
       </c>
       <c r="C56" t="n">
-        <v>0.02996648413848757</v>
+        <v>0.4659516322669067</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -75456,7 +75456,7 @@
         <v>47</v>
       </c>
       <c r="C57" t="n">
-        <v>0.8523502574260395</v>
+        <v>0.7353661059349458</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -75472,7 +75472,7 @@
         <v>11</v>
       </c>
       <c r="C58" t="n">
-        <v>0.9155482011643419</v>
+        <v>0.5682716326989473</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -75488,7 +75488,7 @@
         <v>142</v>
       </c>
       <c r="C59" t="n">
-        <v>0.09814178266734253</v>
+        <v>0.173254614415656</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -75504,7 +75504,7 @@
         <v>143</v>
       </c>
       <c r="C60" t="n">
-        <v>0.1009686949607518</v>
+        <v>0.004113363882196186</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -75520,7 +75520,7 @@
         <v>104</v>
       </c>
       <c r="C61" t="n">
-        <v>0.671167199299765</v>
+        <v>0.8851487458379724</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -75536,7 +75536,7 @@
         <v>117</v>
       </c>
       <c r="C62" t="n">
-        <v>0.5178376977289388</v>
+        <v>0.0144736089294667</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -75552,7 +75552,7 @@
         <v>82</v>
       </c>
       <c r="C63" t="n">
-        <v>0.1311306240832151</v>
+        <v>0.06941184454563465</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -75568,7 +75568,7 @@
         <v>59</v>
       </c>
       <c r="C64" t="n">
-        <v>0.2238165364617548</v>
+        <v>0.2706997963266099</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -75584,7 +75584,7 @@
         <v>142</v>
       </c>
       <c r="C65" t="n">
-        <v>0.4401728178817179</v>
+        <v>0.7215060837037816</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -75600,7 +75600,7 @@
         <v>143</v>
       </c>
       <c r="C66" t="n">
-        <v>0.6994759614138565</v>
+        <v>0.7529013503955737</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -75616,7 +75616,7 @@
         <v>157</v>
       </c>
       <c r="C67" t="n">
-        <v>0.684650534522644</v>
+        <v>0.6237596350052667</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -75632,7 +75632,7 @@
         <v>162</v>
       </c>
       <c r="C68" t="n">
-        <v>0.6376846147801437</v>
+        <v>0.950826788586892</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
@@ -75648,7 +75648,7 @@
         <v>48</v>
       </c>
       <c r="C69" t="n">
-        <v>0.2297471877059954</v>
+        <v>0.2330615523618403</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -75664,7 +75664,7 @@
         <v>110</v>
       </c>
       <c r="C70" t="n">
-        <v>0.8579049714425224</v>
+        <v>0.4109712423381543</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
@@ -75680,7 +75680,7 @@
         <v>157</v>
       </c>
       <c r="C71" t="n">
-        <v>0.7013333581610166</v>
+        <v>0.2627135666224486</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
@@ -75696,7 +75696,7 @@
         <v>48</v>
       </c>
       <c r="C72" t="n">
-        <v>0.5398845980243386</v>
+        <v>0.1937630714442393</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
@@ -75712,7 +75712,7 @@
         <v>142</v>
       </c>
       <c r="C73" t="n">
-        <v>0.7937197492731983</v>
+        <v>0.1834787050105423</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
@@ -75728,7 +75728,7 @@
         <v>143</v>
       </c>
       <c r="C74" t="n">
-        <v>0.8343313375018817</v>
+        <v>0.5223322763225674</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
@@ -75744,7 +75744,7 @@
         <v>110</v>
       </c>
       <c r="C75" t="n">
-        <v>0.7466105013438062</v>
+        <v>0.9315054425114093</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -75760,7 +75760,7 @@
         <v>104</v>
       </c>
       <c r="C76" t="n">
-        <v>0.7202408721531363</v>
+        <v>0.3643930341101366</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
@@ -75776,7 +75776,7 @@
         <v>117</v>
       </c>
       <c r="C77" t="n">
-        <v>0.2932883435734885</v>
+        <v>0.2037158640163097</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
@@ -75792,7 +75792,7 @@
         <v>82</v>
       </c>
       <c r="C78" t="n">
-        <v>0.5994016040765507</v>
+        <v>0.9980349399915378</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -75808,7 +75808,7 @@
         <v>155</v>
       </c>
       <c r="C79" t="n">
-        <v>0.0342216951355665</v>
+        <v>0.8859365599619176</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -75824,7 +75824,7 @@
         <v>162</v>
       </c>
       <c r="C80" t="n">
-        <v>0.8001400936547123</v>
+        <v>0.5305449494666182</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -75840,7 +75840,7 @@
         <v>59</v>
       </c>
       <c r="C81" t="n">
-        <v>0.1339399480406894</v>
+        <v>0.6739129446375158</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
@@ -75856,7 +75856,7 @@
         <v>47</v>
       </c>
       <c r="C82" t="n">
-        <v>0.6329157702135829</v>
+        <v>0.3704087621533132</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -75872,7 +75872,7 @@
         <v>47</v>
       </c>
       <c r="C83" t="n">
-        <v>0.5478922314273286</v>
+        <v>0.1748083003376787</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
@@ -75888,7 +75888,7 @@
         <v>142</v>
       </c>
       <c r="C84" t="n">
-        <v>0.2200461388337077</v>
+        <v>0.2762101138865242</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
@@ -75904,7 +75904,7 @@
         <v>143</v>
       </c>
       <c r="C85" t="n">
-        <v>0.8690027714603886</v>
+        <v>0.01020670963681369</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
@@ -75920,7 +75920,7 @@
         <v>110</v>
       </c>
       <c r="C86" t="n">
-        <v>0.8809330699631144</v>
+        <v>0.4180331347327361</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
@@ -75936,7 +75936,7 @@
         <v>82</v>
       </c>
       <c r="C87" t="n">
-        <v>0.2444611068166471</v>
+        <v>0.3758018092224992</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
@@ -75952,7 +75952,7 @@
         <v>155</v>
       </c>
       <c r="C88" t="n">
-        <v>0.6503882235752688</v>
+        <v>0.1639962557496966</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
@@ -75968,7 +75968,7 @@
         <v>162</v>
       </c>
       <c r="C89" t="n">
-        <v>0.4874433005930867</v>
+        <v>0.5838914143889371</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
@@ -75984,7 +75984,7 @@
         <v>98</v>
       </c>
       <c r="C90" t="n">
-        <v>0.1232915116396951</v>
+        <v>0.4417699386763071</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
@@ -76000,7 +76000,7 @@
         <v>47</v>
       </c>
       <c r="C91" t="n">
-        <v>0.01697924359435299</v>
+        <v>0.1279300652066727</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
@@ -76016,7 +76016,7 @@
         <v>47</v>
       </c>
       <c r="C92" t="n">
-        <v>0.6207262761062605</v>
+        <v>0.7610964521538492</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -76032,7 +76032,7 @@
         <v>140</v>
       </c>
       <c r="C93" t="n">
-        <v>0.09142528501243208</v>
+        <v>0.7283176815800204</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
@@ -76048,7 +76048,7 @@
         <v>143</v>
       </c>
       <c r="C94" t="n">
-        <v>0.0120205098299474</v>
+        <v>0.9817372983273148</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
@@ -76064,7 +76064,7 @@
         <v>110</v>
       </c>
       <c r="C95" t="n">
-        <v>0.7506689176128956</v>
+        <v>0.2889210678398094</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
@@ -76080,7 +76080,7 @@
         <v>155</v>
       </c>
       <c r="C96" t="n">
-        <v>0.64589912528945</v>
+        <v>0.5799654931651665</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
@@ -76096,7 +76096,7 @@
         <v>162</v>
       </c>
       <c r="C97" t="n">
-        <v>0.1854678027584534</v>
+        <v>0.9563140841325163</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
@@ -76112,7 +76112,7 @@
         <v>98</v>
       </c>
       <c r="C98" t="n">
-        <v>0.6504952554291104</v>
+        <v>0.5072017146500765</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
@@ -76128,7 +76128,7 @@
         <v>47</v>
       </c>
       <c r="C99" t="n">
-        <v>0.3729382746041736</v>
+        <v>0.8916217375030169</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
@@ -76144,7 +76144,7 @@
         <v>47</v>
       </c>
       <c r="C100" t="n">
-        <v>0.04402123136740144</v>
+        <v>0.6068023599752768</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
@@ -76160,7 +76160,7 @@
         <v>140</v>
       </c>
       <c r="C101" t="n">
-        <v>0.2199009588515781</v>
+        <v>0.4610026547507756</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
@@ -76176,7 +76176,7 @@
         <v>110</v>
       </c>
       <c r="C102" t="n">
-        <v>0.6594313658152111</v>
+        <v>0.7715473055124493</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
@@ -76192,7 +76192,7 @@
         <v>155</v>
       </c>
       <c r="C103" t="n">
-        <v>0.9629956971511224</v>
+        <v>0.7645752289719404</v>
       </c>
       <c r="D103" t="inlineStr">
         <is>
@@ -76208,7 +76208,7 @@
         <v>98</v>
       </c>
       <c r="C104" t="n">
-        <v>0.8680160885068967</v>
+        <v>0.5855297444970951</v>
       </c>
       <c r="D104" t="inlineStr">
         <is>
@@ -76224,7 +76224,7 @@
         <v>47</v>
       </c>
       <c r="C105" t="n">
-        <v>0.1976559903185351</v>
+        <v>0.08802807106034727</v>
       </c>
       <c r="D105" t="inlineStr">
         <is>
@@ -76240,7 +76240,7 @@
         <v>47</v>
       </c>
       <c r="C106" t="n">
-        <v>0.2321539884699343</v>
+        <v>0.8776183668546258</v>
       </c>
       <c r="D106" t="inlineStr">
         <is>
@@ -76256,7 +76256,7 @@
         <v>140</v>
       </c>
       <c r="C107" t="n">
-        <v>0.7597850049347215</v>
+        <v>0.86995542770435</v>
       </c>
       <c r="D107" t="inlineStr">
         <is>
@@ -76272,7 +76272,7 @@
         <v>11</v>
       </c>
       <c r="C108" t="n">
-        <v>0.9958673884596878</v>
+        <v>0.5741453191042979</v>
       </c>
       <c r="D108" t="inlineStr">
         <is>
@@ -76288,7 +76288,7 @@
         <v>142</v>
       </c>
       <c r="C109" t="n">
-        <v>0.03009343925783636</v>
+        <v>0.8420809802957701</v>
       </c>
       <c r="D109" t="inlineStr">
         <is>
@@ -76304,7 +76304,7 @@
         <v>143</v>
       </c>
       <c r="C110" t="n">
-        <v>0.1408233076469124</v>
+        <v>0.8824142753386158</v>
       </c>
       <c r="D110" t="inlineStr">
         <is>
@@ -76320,7 +76320,7 @@
         <v>104</v>
       </c>
       <c r="C111" t="n">
-        <v>0.5340060438862961</v>
+        <v>0.7781058362665177</v>
       </c>
       <c r="D111" t="inlineStr">
         <is>
@@ -76336,7 +76336,7 @@
         <v>117</v>
       </c>
       <c r="C112" t="n">
-        <v>0.3760853163438075</v>
+        <v>0.8769771406299373</v>
       </c>
       <c r="D112" t="inlineStr">
         <is>
@@ -76352,7 +76352,7 @@
         <v>82</v>
       </c>
       <c r="C113" t="n">
-        <v>0.04442414665791217</v>
+        <v>0.4146177803317209</v>
       </c>
       <c r="D113" t="inlineStr">
         <is>
@@ -76368,7 +76368,7 @@
         <v>59</v>
       </c>
       <c r="C114" t="n">
-        <v>0.7723466071274337</v>
+        <v>0.2168482599469281</v>
       </c>
       <c r="D114" t="inlineStr">
         <is>
@@ -76384,7 +76384,7 @@
         <v>143</v>
       </c>
       <c r="C115" t="n">
-        <v>0.9731967104693098</v>
+        <v>0.9290555567082968</v>
       </c>
       <c r="D115" t="inlineStr">
         <is>
@@ -76400,7 +76400,7 @@
         <v>162</v>
       </c>
       <c r="C116" t="n">
-        <v>0.7067310503302066</v>
+        <v>0.1415672861953875</v>
       </c>
       <c r="D116" t="inlineStr">
         <is>
@@ -76416,7 +76416,7 @@
         <v>142</v>
       </c>
       <c r="C117" t="n">
-        <v>0.04926602711830463</v>
+        <v>0.1846673520379201</v>
       </c>
       <c r="D117" t="inlineStr">
         <is>
@@ -76432,7 +76432,7 @@
         <v>143</v>
       </c>
       <c r="C118" t="n">
-        <v>0.7841605886045731</v>
+        <v>0.8781628861904732</v>
       </c>
       <c r="D118" t="inlineStr">
         <is>
@@ -76448,7 +76448,7 @@
         <v>110</v>
       </c>
       <c r="C119" t="n">
-        <v>0.08967798072124245</v>
+        <v>0.9738031047163868</v>
       </c>
       <c r="D119" t="inlineStr">
         <is>
@@ -76464,7 +76464,7 @@
         <v>157</v>
       </c>
       <c r="C120" t="n">
-        <v>0.1974992282310232</v>
+        <v>0.1321973925621786</v>
       </c>
       <c r="D120" t="inlineStr">
         <is>
@@ -76480,7 +76480,7 @@
         <v>155</v>
       </c>
       <c r="C121" t="n">
-        <v>0.3416820648280253</v>
+        <v>0.8318379842630914</v>
       </c>
       <c r="D121" t="inlineStr">
         <is>
@@ -76496,7 +76496,7 @@
         <v>162</v>
       </c>
       <c r="C122" t="n">
-        <v>0.7089110960359694</v>
+        <v>0.4270472153978369</v>
       </c>
       <c r="D122" t="inlineStr">
         <is>
@@ -76512,7 +76512,7 @@
         <v>98</v>
       </c>
       <c r="C123" t="n">
-        <v>0.04595632340059574</v>
+        <v>0.8877343543525037</v>
       </c>
       <c r="D123" t="inlineStr">
         <is>
@@ -76528,7 +76528,7 @@
         <v>48</v>
       </c>
       <c r="C124" t="n">
-        <v>0.9224548390283255</v>
+        <v>0.4171073088939558</v>
       </c>
       <c r="D124" t="inlineStr">
         <is>
@@ -76544,7 +76544,7 @@
         <v>47</v>
       </c>
       <c r="C125" t="n">
-        <v>0.6559449054120274</v>
+        <v>0.5237785458538796</v>
       </c>
       <c r="D125" t="inlineStr">
         <is>
@@ -76560,7 +76560,7 @@
         <v>47</v>
       </c>
       <c r="C126" t="n">
-        <v>0.8892404635160024</v>
+        <v>0.2498087173041161</v>
       </c>
       <c r="D126" t="inlineStr">
         <is>
@@ -76576,7 +76576,7 @@
         <v>140</v>
       </c>
       <c r="C127" t="n">
-        <v>0.5603906051682567</v>
+        <v>0.04494802958246136</v>
       </c>
       <c r="D127" t="inlineStr">
         <is>
@@ -76592,7 +76592,7 @@
         <v>98</v>
       </c>
       <c r="C128" t="n">
-        <v>0.3307984678382561</v>
+        <v>0.6203939500291505</v>
       </c>
       <c r="D128" t="inlineStr">
         <is>
@@ -76608,7 +76608,7 @@
         <v>140</v>
       </c>
       <c r="C129" t="n">
-        <v>0.005434309393466563</v>
+        <v>0.1261320010172139</v>
       </c>
       <c r="D129" t="inlineStr">
         <is>
@@ -76624,7 +76624,7 @@
         <v>11</v>
       </c>
       <c r="C130" t="n">
-        <v>0.7555819586613384</v>
+        <v>0.1043360903401105</v>
       </c>
       <c r="D130" t="inlineStr">
         <is>
@@ -76640,7 +76640,7 @@
         <v>142</v>
       </c>
       <c r="C131" t="n">
-        <v>0.5562927948038162</v>
+        <v>0.2690233390031389</v>
       </c>
       <c r="D131" t="inlineStr">
         <is>
@@ -76656,7 +76656,7 @@
         <v>143</v>
       </c>
       <c r="C132" t="n">
-        <v>0.9907060843944024</v>
+        <v>0.2741018892819503</v>
       </c>
       <c r="D132" t="inlineStr">
         <is>
@@ -76672,7 +76672,7 @@
         <v>104</v>
       </c>
       <c r="C133" t="n">
-        <v>0.3267240094012124</v>
+        <v>0.4092619117367177</v>
       </c>
       <c r="D133" t="inlineStr">
         <is>
@@ -76688,7 +76688,7 @@
         <v>117</v>
       </c>
       <c r="C134" t="n">
-        <v>7.690986708341896e-05</v>
+        <v>0.1945668746423598</v>
       </c>
       <c r="D134" t="inlineStr">
         <is>
@@ -76704,7 +76704,7 @@
         <v>82</v>
       </c>
       <c r="C135" t="n">
-        <v>0.4875221936365722</v>
+        <v>0.3452265791595139</v>
       </c>
       <c r="D135" t="inlineStr">
         <is>
@@ -76720,7 +76720,7 @@
         <v>155</v>
       </c>
       <c r="C136" t="n">
-        <v>0.6642462840796594</v>
+        <v>0.3334639416288729</v>
       </c>
       <c r="D136" t="inlineStr">
         <is>
@@ -76736,7 +76736,7 @@
         <v>162</v>
       </c>
       <c r="C137" t="n">
-        <v>0.2176761961644801</v>
+        <v>0.2618177690656022</v>
       </c>
       <c r="D137" t="inlineStr">
         <is>
@@ -76752,7 +76752,7 @@
         <v>59</v>
       </c>
       <c r="C138" t="n">
-        <v>0.3974096758500907</v>
+        <v>0.9936900307425973</v>
       </c>
       <c r="D138" t="inlineStr">
         <is>
@@ -76768,7 +76768,7 @@
         <v>47</v>
       </c>
       <c r="C139" t="n">
-        <v>0.6189959831689271</v>
+        <v>0.8822363934604621</v>
       </c>
       <c r="D139" t="inlineStr">
         <is>
@@ -76784,7 +76784,7 @@
         <v>47</v>
       </c>
       <c r="C140" t="n">
-        <v>0.1644107093138756</v>
+        <v>0.08938227193664217</v>
       </c>
       <c r="D140" t="inlineStr">
         <is>
@@ -76800,7 +76800,7 @@
         <v>142</v>
       </c>
       <c r="C141" t="n">
-        <v>0.4242193655533819</v>
+        <v>0.3095735153543542</v>
       </c>
       <c r="D141" t="inlineStr">
         <is>
@@ -76816,7 +76816,7 @@
         <v>157</v>
       </c>
       <c r="C142" t="n">
-        <v>0.7435851386202413</v>
+        <v>0.5570879951934151</v>
       </c>
       <c r="D142" t="inlineStr">
         <is>
@@ -76832,7 +76832,7 @@
         <v>162</v>
       </c>
       <c r="C143" t="n">
-        <v>0.8243644465920228</v>
+        <v>0.9386961053697362</v>
       </c>
       <c r="D143" t="inlineStr">
         <is>
@@ -76848,7 +76848,7 @@
         <v>48</v>
       </c>
       <c r="C144" t="n">
-        <v>0.8724727729512909</v>
+        <v>0.2477861853047865</v>
       </c>
       <c r="D144" t="inlineStr">
         <is>
@@ -76864,7 +76864,7 @@
         <v>143</v>
       </c>
       <c r="C145" t="n">
-        <v>0.2012977852344108</v>
+        <v>0.8749241691216187</v>
       </c>
       <c r="D145" t="inlineStr">
         <is>
@@ -76880,7 +76880,7 @@
         <v>142</v>
       </c>
       <c r="C146" t="n">
-        <v>0.1829551181134852</v>
+        <v>0.7206885265376411</v>
       </c>
       <c r="D146" t="inlineStr">
         <is>
@@ -76896,7 +76896,7 @@
         <v>157</v>
       </c>
       <c r="C147" t="n">
-        <v>0.7020935473567649</v>
+        <v>0.6227784235187332</v>
       </c>
       <c r="D147" t="inlineStr">
         <is>
@@ -76912,7 +76912,7 @@
         <v>48</v>
       </c>
       <c r="C148" t="n">
-        <v>0.7615105337949202</v>
+        <v>0.8885004913866983</v>
       </c>
       <c r="D148" t="inlineStr">
         <is>
@@ -76928,7 +76928,7 @@
         <v>142</v>
       </c>
       <c r="C149" t="n">
-        <v>0.91484323679732</v>
+        <v>0.4961381658136943</v>
       </c>
       <c r="D149" t="inlineStr">
         <is>
@@ -76944,7 +76944,7 @@
         <v>157</v>
       </c>
       <c r="C150" t="n">
-        <v>0.6658253646681518</v>
+        <v>0.5922284460279208</v>
       </c>
       <c r="D150" t="inlineStr">
         <is>
@@ -76960,7 +76960,7 @@
         <v>48</v>
       </c>
       <c r="C151" t="n">
-        <v>0.1577381488005043</v>
+        <v>0.9764806918234951</v>
       </c>
       <c r="D151" t="inlineStr">
         <is>
@@ -76976,7 +76976,7 @@
         <v>142</v>
       </c>
       <c r="C152" t="n">
-        <v>0.267897524332071</v>
+        <v>0.1468143986211824</v>
       </c>
       <c r="D152" t="inlineStr">
         <is>
@@ -76992,7 +76992,7 @@
         <v>143</v>
       </c>
       <c r="C153" t="n">
-        <v>0.04093747691416505</v>
+        <v>0.03830523423871801</v>
       </c>
       <c r="D153" t="inlineStr">
         <is>
@@ -77008,7 +77008,7 @@
         <v>110</v>
       </c>
       <c r="C154" t="n">
-        <v>0.07674108926686907</v>
+        <v>0.6782116103979681</v>
       </c>
       <c r="D154" t="inlineStr">
         <is>
@@ -77024,7 +77024,7 @@
         <v>157</v>
       </c>
       <c r="C155" t="n">
-        <v>0.5332436572590459</v>
+        <v>0.2689255350327576</v>
       </c>
       <c r="D155" t="inlineStr">
         <is>
@@ -77040,7 +77040,7 @@
         <v>155</v>
       </c>
       <c r="C156" t="n">
-        <v>0.1130192208915322</v>
+        <v>0.6073940714659706</v>
       </c>
       <c r="D156" t="inlineStr">
         <is>
@@ -77056,7 +77056,7 @@
         <v>162</v>
       </c>
       <c r="C157" t="n">
-        <v>0.963032048570978</v>
+        <v>0.9381919237310975</v>
       </c>
       <c r="D157" t="inlineStr">
         <is>
@@ -77072,7 +77072,7 @@
         <v>48</v>
       </c>
       <c r="C158" t="n">
-        <v>0.4037931497164181</v>
+        <v>0.07268897572797672</v>
       </c>
       <c r="D158" t="inlineStr">
         <is>
@@ -77088,7 +77088,7 @@
         <v>47</v>
       </c>
       <c r="C159" t="n">
-        <v>0.6189567188095966</v>
+        <v>0.4350442355708004</v>
       </c>
       <c r="D159" t="inlineStr">
         <is>
@@ -77104,7 +77104,7 @@
         <v>47</v>
       </c>
       <c r="C160" t="n">
-        <v>0.2670364676182859</v>
+        <v>0.7173448792164604</v>
       </c>
       <c r="D160" t="inlineStr">
         <is>
@@ -77120,7 +77120,7 @@
         <v>110</v>
       </c>
       <c r="C161" t="n">
-        <v>0.6761104713874739</v>
+        <v>0.3490192427240716</v>
       </c>
       <c r="D161" t="inlineStr">
         <is>
@@ -77136,7 +77136,7 @@
         <v>155</v>
       </c>
       <c r="C162" t="n">
-        <v>0.0004708143739901027</v>
+        <v>0.3142018384563601</v>
       </c>
       <c r="D162" t="inlineStr">
         <is>
@@ -77152,7 +77152,7 @@
         <v>162</v>
       </c>
       <c r="C163" t="n">
-        <v>0.6461277086754287</v>
+        <v>0.443936338719359</v>
       </c>
       <c r="D163" t="inlineStr">
         <is>
@@ -77168,7 +77168,7 @@
         <v>98</v>
       </c>
       <c r="C164" t="n">
-        <v>0.9019144578008932</v>
+        <v>0.3239856623827155</v>
       </c>
       <c r="D164" t="inlineStr">
         <is>
@@ -77184,7 +77184,7 @@
         <v>47</v>
       </c>
       <c r="C165" t="n">
-        <v>0.2506267800994048</v>
+        <v>0.3398165961832856</v>
       </c>
       <c r="D165" t="inlineStr">
         <is>
@@ -77200,7 +77200,7 @@
         <v>47</v>
       </c>
       <c r="C166" t="n">
-        <v>0.2836985632688901</v>
+        <v>0.5074185249380916</v>
       </c>
       <c r="D166" t="inlineStr">
         <is>
@@ -77216,7 +77216,7 @@
         <v>140</v>
       </c>
       <c r="C167" t="n">
-        <v>0.7003927227009508</v>
+        <v>0.808760629257246</v>
       </c>
       <c r="D167" t="inlineStr">
         <is>
@@ -77232,7 +77232,7 @@
         <v>143</v>
       </c>
       <c r="C168" t="n">
-        <v>0.8920236346622883</v>
+        <v>0.05575993558746062</v>
       </c>
       <c r="D168" t="inlineStr">
         <is>
@@ -77248,7 +77248,7 @@
         <v>11</v>
       </c>
       <c r="C169" t="n">
-        <v>0.6879010524945844</v>
+        <v>0.2971136214434705</v>
       </c>
       <c r="D169" t="inlineStr">
         <is>
@@ -77264,7 +77264,7 @@
         <v>142</v>
       </c>
       <c r="C170" t="n">
-        <v>0.3094643244287109</v>
+        <v>0.6553915975968349</v>
       </c>
       <c r="D170" t="inlineStr">
         <is>
@@ -77280,7 +77280,7 @@
         <v>143</v>
       </c>
       <c r="C171" t="n">
-        <v>0.2641794967190125</v>
+        <v>0.1092380534343119</v>
       </c>
       <c r="D171" t="inlineStr">
         <is>
@@ -77296,7 +77296,7 @@
         <v>110</v>
       </c>
       <c r="C172" t="n">
-        <v>0.7433505933468242</v>
+        <v>0.2465175433650472</v>
       </c>
       <c r="D172" t="inlineStr">
         <is>
@@ -77312,7 +77312,7 @@
         <v>104</v>
       </c>
       <c r="C173" t="n">
-        <v>0.4476958000994171</v>
+        <v>0.6415259690667195</v>
       </c>
       <c r="D173" t="inlineStr">
         <is>
@@ -77328,7 +77328,7 @@
         <v>117</v>
       </c>
       <c r="C174" t="n">
-        <v>0.7062523921391383</v>
+        <v>0.9165370767862362</v>
       </c>
       <c r="D174" t="inlineStr">
         <is>
@@ -77344,7 +77344,7 @@
         <v>82</v>
       </c>
       <c r="C175" t="n">
-        <v>0.1159366187036077</v>
+        <v>0.2717916957745122</v>
       </c>
       <c r="D175" t="inlineStr">
         <is>
@@ -77360,7 +77360,7 @@
         <v>155</v>
       </c>
       <c r="C176" t="n">
-        <v>0.1069463307471825</v>
+        <v>0.8976392933301562</v>
       </c>
       <c r="D176" t="inlineStr">
         <is>
@@ -77376,7 +77376,7 @@
         <v>162</v>
       </c>
       <c r="C177" t="n">
-        <v>0.8209848781406418</v>
+        <v>0.4842775153105624</v>
       </c>
       <c r="D177" t="inlineStr">
         <is>
@@ -77392,7 +77392,7 @@
         <v>59</v>
       </c>
       <c r="C178" t="n">
-        <v>0.07203687079380305</v>
+        <v>0.3549036687899779</v>
       </c>
       <c r="D178" t="inlineStr">
         <is>
@@ -77408,7 +77408,7 @@
         <v>47</v>
       </c>
       <c r="C179" t="n">
-        <v>0.3567350726359461</v>
+        <v>0.508046167919956</v>
       </c>
       <c r="D179" t="inlineStr">
         <is>
@@ -77424,7 +77424,7 @@
         <v>47</v>
       </c>
       <c r="C180" t="n">
-        <v>0.1130161169695801</v>
+        <v>0.6578288856033909</v>
       </c>
       <c r="D180" t="inlineStr">
         <is>
@@ -77440,7 +77440,7 @@
         <v>77</v>
       </c>
       <c r="C181" t="n">
-        <v>0.4066621566362434</v>
+        <v>0.8730596353013093</v>
       </c>
       <c r="D181" t="inlineStr">
         <is>
@@ -77456,7 +77456,7 @@
         <v>54</v>
       </c>
       <c r="C182" t="n">
-        <v>0.4356061465163669</v>
+        <v>0.2513599600136442</v>
       </c>
       <c r="D182" t="inlineStr">
         <is>
@@ -77472,7 +77472,7 @@
         <v>92</v>
       </c>
       <c r="C183" t="n">
-        <v>0.456381748132473</v>
+        <v>0.9483246865110212</v>
       </c>
       <c r="D183" t="inlineStr">
         <is>
@@ -77488,7 +77488,7 @@
         <v>104</v>
       </c>
       <c r="C184" t="n">
-        <v>0.7275764533921451</v>
+        <v>0.8558895599754356</v>
       </c>
       <c r="D184" t="inlineStr">
         <is>
@@ -77504,7 +77504,7 @@
         <v>48</v>
       </c>
       <c r="C185" t="n">
-        <v>0.4612772554058088</v>
+        <v>0.1180100775014203</v>
       </c>
       <c r="D185" t="inlineStr">
         <is>
@@ -77520,7 +77520,7 @@
         <v>104</v>
       </c>
       <c r="C186" t="n">
-        <v>0.2488897169636842</v>
+        <v>0.5311699313777396</v>
       </c>
       <c r="D186" t="inlineStr">
         <is>
@@ -77536,7 +77536,7 @@
         <v>95</v>
       </c>
       <c r="C187" t="n">
-        <v>0.7545041986175571</v>
+        <v>0.1614017197010297</v>
       </c>
       <c r="D187" t="inlineStr">
         <is>
@@ -77552,7 +77552,7 @@
         <v>52</v>
       </c>
       <c r="C188" t="n">
-        <v>0.7007145219817772</v>
+        <v>0.5165125575334888</v>
       </c>
       <c r="D188" t="inlineStr">
         <is>
@@ -77568,7 +77568,7 @@
         <v>104</v>
       </c>
       <c r="C189" t="n">
-        <v>0.9238610226853764</v>
+        <v>0.2852305086978408</v>
       </c>
       <c r="D189" t="inlineStr">
         <is>
@@ -77584,7 +77584,7 @@
         <v>79</v>
       </c>
       <c r="C190" t="n">
-        <v>0.6144904647510775</v>
+        <v>0.2817161662278701</v>
       </c>
       <c r="D190" t="inlineStr">
         <is>
@@ -77600,7 +77600,7 @@
         <v>104</v>
       </c>
       <c r="C191" t="n">
-        <v>0.5444766462791988</v>
+        <v>0.1914852354797859</v>
       </c>
       <c r="D191" t="inlineStr">
         <is>
@@ -77616,7 +77616,7 @@
         <v>59</v>
       </c>
       <c r="C192" t="n">
-        <v>0.3160141365780198</v>
+        <v>0.1331879923207211</v>
       </c>
       <c r="D192" t="inlineStr">
         <is>
@@ -77632,7 +77632,7 @@
         <v>112</v>
       </c>
       <c r="C193" t="n">
-        <v>0.5613554701102333</v>
+        <v>0.4404614883624772</v>
       </c>
       <c r="D193" t="inlineStr">
         <is>
@@ -77648,7 +77648,7 @@
         <v>74</v>
       </c>
       <c r="C194" t="n">
-        <v>0.1436912751371717</v>
+        <v>0.02108095022182854</v>
       </c>
       <c r="D194" t="inlineStr">
         <is>
@@ -77664,7 +77664,7 @@
         <v>104</v>
       </c>
       <c r="C195" t="n">
-        <v>0.1087160855115499</v>
+        <v>0.8693007417571734</v>
       </c>
       <c r="D195" t="inlineStr">
         <is>
@@ -77680,7 +77680,7 @@
         <v>143</v>
       </c>
       <c r="C196" t="n">
-        <v>0.676463167843932</v>
+        <v>0.3098128742876638</v>
       </c>
       <c r="D196" t="inlineStr">
         <is>
@@ -77696,7 +77696,7 @@
         <v>143</v>
       </c>
       <c r="C197" t="n">
-        <v>0.7439486846335001</v>
+        <v>0.0735580963721818</v>
       </c>
       <c r="D197" t="inlineStr">
         <is>
@@ -77712,7 +77712,7 @@
         <v>143</v>
       </c>
       <c r="C198" t="n">
-        <v>0.2689882374801655</v>
+        <v>0.4407984755224235</v>
       </c>
       <c r="D198" t="inlineStr">
         <is>
@@ -77728,7 +77728,7 @@
         <v>143</v>
       </c>
       <c r="C199" t="n">
-        <v>0.9464818631257567</v>
+        <v>0.117281493528317</v>
       </c>
       <c r="D199" t="inlineStr">
         <is>
@@ -77744,7 +77744,7 @@
         <v>103</v>
       </c>
       <c r="C200" t="n">
-        <v>0.7921254475767989</v>
+        <v>0.7400294530593045</v>
       </c>
       <c r="D200" t="inlineStr">
         <is>
@@ -77760,7 +77760,7 @@
         <v>146</v>
       </c>
       <c r="C201" t="n">
-        <v>0.1366136760249643</v>
+        <v>0.0778833536584328</v>
       </c>
       <c r="D201" t="inlineStr">
         <is>
@@ -77776,7 +77776,7 @@
         <v>104</v>
       </c>
       <c r="C202" t="n">
-        <v>0.9370445962633214</v>
+        <v>0.6181802703364215</v>
       </c>
       <c r="D202" t="inlineStr">
         <is>
@@ -77792,7 +77792,7 @@
         <v>104</v>
       </c>
       <c r="C203" t="n">
-        <v>0.3940720079959363</v>
+        <v>0.9574688219677693</v>
       </c>
       <c r="D203" t="inlineStr">
         <is>
@@ -77808,7 +77808,7 @@
         <v>41</v>
       </c>
       <c r="C204" t="n">
-        <v>0.8373932473271044</v>
+        <v>0.8165497977965889</v>
       </c>
       <c r="D204" t="inlineStr">
         <is>
@@ -77824,7 +77824,7 @@
         <v>147</v>
       </c>
       <c r="C205" t="n">
-        <v>0.6304520098004535</v>
+        <v>0.5282687115715108</v>
       </c>
       <c r="D205" t="inlineStr">
         <is>
@@ -77840,7 +77840,7 @@
         <v>125</v>
       </c>
       <c r="C206" t="n">
-        <v>0.09846998496078474</v>
+        <v>0.941669693573897</v>
       </c>
       <c r="D206" t="inlineStr">
         <is>
@@ -77856,7 +77856,7 @@
         <v>51</v>
       </c>
       <c r="C207" t="n">
-        <v>0.4715635719276083</v>
+        <v>0.638621606746978</v>
       </c>
       <c r="D207" t="inlineStr">
         <is>
@@ -77872,7 +77872,7 @@
         <v>51</v>
       </c>
       <c r="C208" t="n">
-        <v>0.5322831404590729</v>
+        <v>0.03085966149212049</v>
       </c>
       <c r="D208" t="inlineStr">
         <is>
@@ -77888,7 +77888,7 @@
         <v>51</v>
       </c>
       <c r="C209" t="n">
-        <v>0.931017608150802</v>
+        <v>0.1094889113174242</v>
       </c>
       <c r="D209" t="inlineStr">
         <is>
@@ -77904,7 +77904,7 @@
         <v>50</v>
       </c>
       <c r="C210" t="n">
-        <v>0.4253754168117553</v>
+        <v>0.6159630529599615</v>
       </c>
       <c r="D210" t="inlineStr">
         <is>
@@ -77920,7 +77920,7 @@
         <v>124</v>
       </c>
       <c r="C211" t="n">
-        <v>0.984184155260511</v>
+        <v>0.7951848619916208</v>
       </c>
       <c r="D211" t="inlineStr">
         <is>
@@ -77936,7 +77936,7 @@
         <v>26</v>
       </c>
       <c r="C212" t="n">
-        <v>0.1626604319533177</v>
+        <v>0.8612469085599121</v>
       </c>
       <c r="D212" t="inlineStr">
         <is>
@@ -77952,7 +77952,7 @@
         <v>125</v>
       </c>
       <c r="C213" t="n">
-        <v>0.1459398054040442</v>
+        <v>0.1021012336725244</v>
       </c>
       <c r="D213" t="inlineStr">
         <is>
@@ -77968,7 +77968,7 @@
         <v>136</v>
       </c>
       <c r="C214" t="n">
-        <v>0.8823312167394973</v>
+        <v>0.2297507098876735</v>
       </c>
       <c r="D214" t="inlineStr">
         <is>
@@ -77984,7 +77984,7 @@
         <v>11</v>
       </c>
       <c r="C215" t="n">
-        <v>0.9862362968480357</v>
+        <v>0.6977242960441433</v>
       </c>
       <c r="D215" t="inlineStr">
         <is>
@@ -78000,7 +78000,7 @@
         <v>68</v>
       </c>
       <c r="C216" t="n">
-        <v>0.3181772696908467</v>
+        <v>0.2164710831915582</v>
       </c>
       <c r="D216" t="inlineStr">
         <is>
@@ -78016,7 +78016,7 @@
         <v>161</v>
       </c>
       <c r="C217" t="n">
-        <v>0.8523399086006601</v>
+        <v>0.2645748508920125</v>
       </c>
       <c r="D217" t="inlineStr">
         <is>
@@ -78032,7 +78032,7 @@
         <v>3</v>
       </c>
       <c r="C218" t="n">
-        <v>0.1292120397565104</v>
+        <v>0.8309898923929621</v>
       </c>
       <c r="D218" t="inlineStr">
         <is>
@@ -78048,7 +78048,7 @@
         <v>50</v>
       </c>
       <c r="C219" t="n">
-        <v>0.3207715284599644</v>
+        <v>0.7977083407575372</v>
       </c>
       <c r="D219" t="inlineStr">
         <is>
@@ -78064,7 +78064,7 @@
         <v>140</v>
       </c>
       <c r="C220" t="n">
-        <v>0.6389520846307246</v>
+        <v>0.8977783105286391</v>
       </c>
       <c r="D220" t="inlineStr">
         <is>
@@ -78080,7 +78080,7 @@
         <v>120</v>
       </c>
       <c r="C221" t="n">
-        <v>0.5634615156238844</v>
+        <v>0.1355547115954544</v>
       </c>
       <c r="D221" t="inlineStr">
         <is>
@@ -78096,7 +78096,7 @@
         <v>130</v>
       </c>
       <c r="C222" t="n">
-        <v>0.1369143975171424</v>
+        <v>0.415834882020193</v>
       </c>
       <c r="D222" t="inlineStr">
         <is>
@@ -78112,7 +78112,7 @@
         <v>142</v>
       </c>
       <c r="C223" t="n">
-        <v>0.357549104331697</v>
+        <v>0.01694980975692073</v>
       </c>
       <c r="D223" t="inlineStr">
         <is>
@@ -78128,7 +78128,7 @@
         <v>142</v>
       </c>
       <c r="C224" t="n">
-        <v>0.5485744899607571</v>
+        <v>0.7709815290332479</v>
       </c>
       <c r="D224" t="inlineStr">
         <is>
@@ -78144,7 +78144,7 @@
         <v>142</v>
       </c>
       <c r="C225" t="n">
-        <v>0.8216532719096538</v>
+        <v>0.9602397355761789</v>
       </c>
       <c r="D225" t="inlineStr">
         <is>
@@ -78160,7 +78160,7 @@
         <v>142</v>
       </c>
       <c r="C226" t="n">
-        <v>0.1410478285523385</v>
+        <v>0.8588810597816581</v>
       </c>
       <c r="D226" t="inlineStr">
         <is>
@@ -78170,13 +78170,13 @@
     </row>
     <row r="227">
       <c r="A227" t="n">
-        <v>147</v>
+        <v>52</v>
       </c>
       <c r="B227" t="n">
         <v>142</v>
       </c>
       <c r="C227" t="n">
-        <v>0.4035322128363371</v>
+        <v>0.5175146758091683</v>
       </c>
       <c r="D227" t="inlineStr">
         <is>
@@ -78186,13 +78186,13 @@
     </row>
     <row r="228">
       <c r="A228" t="n">
-        <v>52</v>
+        <v>143</v>
       </c>
       <c r="B228" t="n">
         <v>142</v>
       </c>
       <c r="C228" t="n">
-        <v>0.8917972400891955</v>
+        <v>0.3532136081221946</v>
       </c>
       <c r="D228" t="inlineStr">
         <is>
@@ -78202,13 +78202,13 @@
     </row>
     <row r="229">
       <c r="A229" t="n">
-        <v>121</v>
+        <v>34</v>
       </c>
       <c r="B229" t="n">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C229" t="n">
-        <v>0.9849390395157808</v>
+        <v>0.4105083024150072</v>
       </c>
       <c r="D229" t="inlineStr">
         <is>
@@ -78218,13 +78218,13 @@
     </row>
     <row r="230">
       <c r="A230" t="n">
+        <v>104</v>
+      </c>
+      <c r="B230" t="n">
         <v>143</v>
       </c>
-      <c r="B230" t="n">
-        <v>142</v>
-      </c>
       <c r="C230" t="n">
-        <v>0.4355723165053778</v>
+        <v>0.9014305001125518</v>
       </c>
       <c r="D230" t="inlineStr">
         <is>
@@ -78234,13 +78234,13 @@
     </row>
     <row r="231">
       <c r="A231" t="n">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="B231" t="n">
         <v>143</v>
       </c>
       <c r="C231" t="n">
-        <v>0.9360864377696096</v>
+        <v>0.2547481414612452</v>
       </c>
       <c r="D231" t="inlineStr">
         <is>
@@ -78250,13 +78250,13 @@
     </row>
     <row r="232">
       <c r="A232" t="n">
+        <v>128</v>
+      </c>
+      <c r="B232" t="n">
         <v>104</v>
       </c>
-      <c r="B232" t="n">
-        <v>143</v>
-      </c>
       <c r="C232" t="n">
-        <v>0.7667594615564153</v>
+        <v>0.3756633817676911</v>
       </c>
       <c r="D232" t="inlineStr">
         <is>
@@ -78266,13 +78266,13 @@
     </row>
     <row r="233">
       <c r="A233" t="n">
-        <v>128</v>
+        <v>52</v>
       </c>
       <c r="B233" t="n">
-        <v>143</v>
+        <v>104</v>
       </c>
       <c r="C233" t="n">
-        <v>0.7971429498853904</v>
+        <v>0.9715462934582937</v>
       </c>
       <c r="D233" t="inlineStr">
         <is>
@@ -78282,13 +78282,13 @@
     </row>
     <row r="234">
       <c r="A234" t="n">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="B234" t="n">
-        <v>143</v>
+        <v>104</v>
       </c>
       <c r="C234" t="n">
-        <v>0.05210000167148654</v>
+        <v>0.6901860142878667</v>
       </c>
       <c r="D234" t="inlineStr">
         <is>
@@ -78298,13 +78298,13 @@
     </row>
     <row r="235">
       <c r="A235" t="n">
-        <v>147</v>
+        <v>34</v>
       </c>
       <c r="B235" t="n">
-        <v>143</v>
+        <v>70</v>
       </c>
       <c r="C235" t="n">
-        <v>0.3152946906388545</v>
+        <v>0.07611810124329266</v>
       </c>
       <c r="D235" t="inlineStr">
         <is>
@@ -78314,13 +78314,13 @@
     </row>
     <row r="236">
       <c r="A236" t="n">
-        <v>52</v>
+        <v>104</v>
       </c>
       <c r="B236" t="n">
-        <v>143</v>
+        <v>70</v>
       </c>
       <c r="C236" t="n">
-        <v>0.01048396140172869</v>
+        <v>0.1396454692015702</v>
       </c>
       <c r="D236" t="inlineStr">
         <is>
@@ -78330,13 +78330,13 @@
     </row>
     <row r="237">
       <c r="A237" t="n">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="B237" t="n">
-        <v>143</v>
+        <v>70</v>
       </c>
       <c r="C237" t="n">
-        <v>0.9303542887408164</v>
+        <v>0.5458940659020396</v>
       </c>
       <c r="D237" t="inlineStr">
         <is>
@@ -78346,13 +78346,13 @@
     </row>
     <row r="238">
       <c r="A238" t="n">
-        <v>128</v>
+        <v>147</v>
       </c>
       <c r="B238" t="n">
-        <v>104</v>
+        <v>70</v>
       </c>
       <c r="C238" t="n">
-        <v>0.4263590119122385</v>
+        <v>0.6215736922490999</v>
       </c>
       <c r="D238" t="inlineStr">
         <is>
@@ -78362,13 +78362,13 @@
     </row>
     <row r="239">
       <c r="A239" t="n">
-        <v>147</v>
+        <v>52</v>
       </c>
       <c r="B239" t="n">
-        <v>104</v>
+        <v>70</v>
       </c>
       <c r="C239" t="n">
-        <v>0.2133949400909111</v>
+        <v>0.7068286957667717</v>
       </c>
       <c r="D239" t="inlineStr">
         <is>
@@ -78378,13 +78378,13 @@
     </row>
     <row r="240">
       <c r="A240" t="n">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="B240" t="n">
-        <v>104</v>
+        <v>70</v>
       </c>
       <c r="C240" t="n">
-        <v>0.468235524148194</v>
+        <v>0.5775363163776921</v>
       </c>
       <c r="D240" t="inlineStr">
         <is>
@@ -78394,321 +78394,321 @@
     </row>
     <row r="241">
       <c r="A241" t="n">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="B241" t="n">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="C241" t="n">
-        <v>0.2595783262861526</v>
+        <v>0.2019406281190083</v>
       </c>
       <c r="D241" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>bituminous</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="n">
-        <v>143</v>
+        <v>34</v>
       </c>
       <c r="B242" t="n">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="C242" t="n">
-        <v>0.1924355725703261</v>
+        <v>0.4917044341398747</v>
       </c>
       <c r="D242" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>bituminous</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="n">
-        <v>48</v>
+        <v>104</v>
       </c>
       <c r="B243" t="n">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="C243" t="n">
-        <v>0.848233813851518</v>
+        <v>0.7991220189689617</v>
       </c>
       <c r="D243" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>bituminous</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="n">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="B244" t="n">
-        <v>70</v>
+        <v>117</v>
       </c>
       <c r="C244" t="n">
-        <v>0.6443685295222136</v>
+        <v>0.3197948299428239</v>
       </c>
       <c r="D244" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>bituminous</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="n">
-        <v>34</v>
+        <v>147</v>
       </c>
       <c r="B245" t="n">
-        <v>70</v>
+        <v>117</v>
       </c>
       <c r="C245" t="n">
-        <v>0.7561101826237737</v>
+        <v>0.3085296614122948</v>
       </c>
       <c r="D245" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>bituminous</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="n">
-        <v>104</v>
+        <v>52</v>
       </c>
       <c r="B246" t="n">
-        <v>70</v>
+        <v>117</v>
       </c>
       <c r="C246" t="n">
-        <v>0.08623072068825677</v>
+        <v>0.8821160716845039</v>
       </c>
       <c r="D246" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>bituminous</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="n">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B247" t="n">
-        <v>70</v>
+        <v>117</v>
       </c>
       <c r="C247" t="n">
-        <v>0.9682357603929912</v>
+        <v>0.2081292296401791</v>
       </c>
       <c r="D247" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>bituminous</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="n">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B248" t="n">
-        <v>70</v>
+        <v>117</v>
       </c>
       <c r="C248" t="n">
-        <v>0.6841831418106209</v>
+        <v>0.5003797637086139</v>
       </c>
       <c r="D248" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>bituminous</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="n">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B249" t="n">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C249" t="n">
-        <v>0.9775585012496232</v>
+        <v>0.2517009780894776</v>
       </c>
       <c r="D249" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>lignite</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="n">
-        <v>121</v>
+        <v>34</v>
       </c>
       <c r="B250" t="n">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="C250" t="n">
-        <v>0.6646026068978587</v>
+        <v>0.2953499734057194</v>
       </c>
       <c r="D250" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>subbituminous</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="n">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="B251" t="n">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="C251" t="n">
-        <v>0.652482336540758</v>
+        <v>0.3924753198848933</v>
       </c>
       <c r="D251" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>subbituminous</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="n">
-        <v>146</v>
+        <v>48</v>
       </c>
       <c r="B252" t="n">
-        <v>117</v>
+        <v>11</v>
       </c>
       <c r="C252" t="n">
-        <v>0.4880270083648099</v>
+        <v>0.5850988487613482</v>
       </c>
       <c r="D252" t="inlineStr">
         <is>
-          <t>bituminous</t>
+          <t>subbituminous</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="n">
-        <v>34</v>
+        <v>146</v>
       </c>
       <c r="B253" t="n">
-        <v>117</v>
+        <v>82</v>
       </c>
       <c r="C253" t="n">
-        <v>0.5536510705046204</v>
+        <v>0.490206137879364</v>
       </c>
       <c r="D253" t="inlineStr">
         <is>
-          <t>bituminous</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="n">
-        <v>104</v>
+        <v>34</v>
       </c>
       <c r="B254" t="n">
-        <v>117</v>
+        <v>82</v>
       </c>
       <c r="C254" t="n">
-        <v>0.2714581556491489</v>
+        <v>0.04386667524703769</v>
       </c>
       <c r="D254" t="inlineStr">
         <is>
-          <t>bituminous</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="n">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="B255" t="n">
-        <v>117</v>
+        <v>82</v>
       </c>
       <c r="C255" t="n">
-        <v>0.3326742436825146</v>
+        <v>0.722733706177471</v>
       </c>
       <c r="D255" t="inlineStr">
         <is>
-          <t>bituminous</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="n">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="B256" t="n">
-        <v>117</v>
+        <v>82</v>
       </c>
       <c r="C256" t="n">
-        <v>0.1743445304288809</v>
+        <v>0.219905477594641</v>
       </c>
       <c r="D256" t="inlineStr">
         <is>
-          <t>bituminous</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="n">
-        <v>52</v>
+        <v>147</v>
       </c>
       <c r="B257" t="n">
-        <v>117</v>
+        <v>82</v>
       </c>
       <c r="C257" t="n">
-        <v>0.7699999823577414</v>
+        <v>0.8026772255989811</v>
       </c>
       <c r="D257" t="inlineStr">
         <is>
-          <t>bituminous</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="n">
-        <v>121</v>
+        <v>52</v>
       </c>
       <c r="B258" t="n">
-        <v>117</v>
+        <v>82</v>
       </c>
       <c r="C258" t="n">
-        <v>0.7457731443220694</v>
+        <v>0.6828303158782532</v>
       </c>
       <c r="D258" t="inlineStr">
         <is>
-          <t>bituminous</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="n">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="B259" t="n">
-        <v>117</v>
+        <v>82</v>
       </c>
       <c r="C259" t="n">
-        <v>0.2759906506251928</v>
+        <v>0.455154424957193</v>
       </c>
       <c r="D259" t="inlineStr">
         <is>
-          <t>bituminous</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="n">
-        <v>48</v>
+        <v>143</v>
       </c>
       <c r="B260" t="n">
-        <v>117</v>
+        <v>82</v>
       </c>
       <c r="C260" t="n">
-        <v>0.09758812961874264</v>
+        <v>0.5476043590456187</v>
       </c>
       <c r="D260" t="inlineStr">
         <is>
-          <t>bituminous</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
@@ -78717,158 +78717,158 @@
         <v>34</v>
       </c>
       <c r="B261" t="n">
-        <v>73</v>
+        <v>21</v>
       </c>
       <c r="C261" t="n">
-        <v>0.4641887253953355</v>
+        <v>0.08067319429163999</v>
       </c>
       <c r="D261" t="inlineStr">
         <is>
-          <t>lignite</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="n">
-        <v>48</v>
+        <v>128</v>
       </c>
       <c r="B262" t="n">
-        <v>73</v>
+        <v>21</v>
       </c>
       <c r="C262" t="n">
-        <v>0.242833977317653</v>
+        <v>0.3485391670849658</v>
       </c>
       <c r="D262" t="inlineStr">
         <is>
-          <t>lignite</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="n">
-        <v>146</v>
+        <v>52</v>
       </c>
       <c r="B263" t="n">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C263" t="n">
-        <v>0.8072700164228278</v>
+        <v>0.9103659272442051</v>
       </c>
       <c r="D263" t="inlineStr">
         <is>
-          <t>subbituminous</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="n">
-        <v>34</v>
+        <v>104</v>
       </c>
       <c r="B264" t="n">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C264" t="n">
-        <v>0.4371384139548581</v>
+        <v>0.8120879239782528</v>
       </c>
       <c r="D264" t="inlineStr">
         <is>
-          <t>subbituminous</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="n">
-        <v>104</v>
+        <v>146</v>
       </c>
       <c r="B265" t="n">
-        <v>11</v>
+        <v>155</v>
       </c>
       <c r="C265" t="n">
-        <v>0.871234593324798</v>
+        <v>0.3688977407090803</v>
       </c>
       <c r="D265" t="inlineStr">
         <is>
-          <t>subbituminous</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="n">
-        <v>128</v>
+        <v>103</v>
       </c>
       <c r="B266" t="n">
-        <v>11</v>
+        <v>155</v>
       </c>
       <c r="C266" t="n">
-        <v>0.5511665752497725</v>
+        <v>0.09673387262431854</v>
       </c>
       <c r="D266" t="inlineStr">
         <is>
-          <t>subbituminous</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="n">
-        <v>52</v>
+        <v>143</v>
       </c>
       <c r="B267" t="n">
-        <v>11</v>
+        <v>155</v>
       </c>
       <c r="C267" t="n">
-        <v>0.4533421355337678</v>
+        <v>0.151451410479381</v>
       </c>
       <c r="D267" t="inlineStr">
         <is>
-          <t>subbituminous</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="n">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B268" t="n">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="C268" t="n">
-        <v>0.7440968287439605</v>
+        <v>0.4493384847146307</v>
       </c>
       <c r="D268" t="inlineStr">
         <is>
-          <t>subbituminous</t>
+          <t>bituminous</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="n">
-        <v>48</v>
+        <v>143</v>
       </c>
       <c r="B269" t="n">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="C269" t="n">
-        <v>0.5084594832567794</v>
+        <v>0.6048259251711993</v>
       </c>
       <c r="D269" t="inlineStr">
         <is>
-          <t>subbituminous</t>
+          <t>bituminous</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="n">
-        <v>146</v>
+        <v>48</v>
       </c>
       <c r="B270" t="n">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="C270" t="n">
-        <v>0.1756364346136945</v>
+        <v>0.4353702399054609</v>
       </c>
       <c r="D270" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>bituminous</t>
         </is>
       </c>
     </row>
@@ -78877,10 +78877,10 @@
         <v>34</v>
       </c>
       <c r="B271" t="n">
-        <v>82</v>
+        <v>152</v>
       </c>
       <c r="C271" t="n">
-        <v>0.3221775137107089</v>
+        <v>0.2391614181953395</v>
       </c>
       <c r="D271" t="inlineStr">
         <is>
@@ -78893,10 +78893,10 @@
         <v>104</v>
       </c>
       <c r="B272" t="n">
-        <v>82</v>
+        <v>152</v>
       </c>
       <c r="C272" t="n">
-        <v>0.4115313843010191</v>
+        <v>0.8510582037061152</v>
       </c>
       <c r="D272" t="inlineStr">
         <is>
@@ -78909,10 +78909,10 @@
         <v>128</v>
       </c>
       <c r="B273" t="n">
-        <v>82</v>
+        <v>152</v>
       </c>
       <c r="C273" t="n">
-        <v>0.6195145283696253</v>
+        <v>0.01014511125394957</v>
       </c>
       <c r="D273" t="inlineStr">
         <is>
@@ -78922,13 +78922,13 @@
     </row>
     <row r="274">
       <c r="A274" t="n">
-        <v>147</v>
+        <v>52</v>
       </c>
       <c r="B274" t="n">
-        <v>82</v>
+        <v>152</v>
       </c>
       <c r="C274" t="n">
-        <v>0.1886269326206115</v>
+        <v>0.2728739919073587</v>
       </c>
       <c r="D274" t="inlineStr">
         <is>
@@ -78938,13 +78938,13 @@
     </row>
     <row r="275">
       <c r="A275" t="n">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="B275" t="n">
-        <v>82</v>
+        <v>152</v>
       </c>
       <c r="C275" t="n">
-        <v>0.7246893181173467</v>
+        <v>0.317708656772082</v>
       </c>
       <c r="D275" t="inlineStr">
         <is>
@@ -78954,13 +78954,13 @@
     </row>
     <row r="276">
       <c r="A276" t="n">
-        <v>121</v>
+        <v>147</v>
       </c>
       <c r="B276" t="n">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="C276" t="n">
-        <v>0.8085429300033465</v>
+        <v>0.945701063183663</v>
       </c>
       <c r="D276" t="inlineStr">
         <is>
@@ -78970,13 +78970,13 @@
     </row>
     <row r="277">
       <c r="A277" t="n">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="B277" t="n">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="C277" t="n">
-        <v>0.4234544163197899</v>
+        <v>0.9959726862277197</v>
       </c>
       <c r="D277" t="inlineStr">
         <is>
@@ -78986,61 +78986,61 @@
     </row>
     <row r="278">
       <c r="A278" t="n">
-        <v>48</v>
+        <v>146</v>
       </c>
       <c r="B278" t="n">
-        <v>82</v>
+        <v>47</v>
       </c>
       <c r="C278" t="n">
-        <v>0.3791966455373288</v>
+        <v>0.08670351739596494</v>
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>bituminous</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="n">
-        <v>146</v>
+        <v>103</v>
       </c>
       <c r="B279" t="n">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="C279" t="n">
-        <v>0.2799955369300978</v>
+        <v>0.7158596320699213</v>
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>bituminous</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="n">
-        <v>34</v>
+        <v>143</v>
       </c>
       <c r="B280" t="n">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="C280" t="n">
-        <v>0.4562385450319423</v>
+        <v>0.530870359970943</v>
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>bituminous</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="n">
-        <v>104</v>
+        <v>146</v>
       </c>
       <c r="B281" t="n">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="C281" t="n">
-        <v>0.7268129385223074</v>
+        <v>0.7121543817301682</v>
       </c>
       <c r="D281" t="inlineStr">
         <is>
@@ -79050,13 +79050,13 @@
     </row>
     <row r="282">
       <c r="A282" t="n">
-        <v>128</v>
+        <v>34</v>
       </c>
       <c r="B282" t="n">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="C282" t="n">
-        <v>0.9665088445793817</v>
+        <v>0.6763600630805685</v>
       </c>
       <c r="D282" t="inlineStr">
         <is>
@@ -79066,13 +79066,13 @@
     </row>
     <row r="283">
       <c r="A283" t="n">
-        <v>147</v>
+        <v>104</v>
       </c>
       <c r="B283" t="n">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="C283" t="n">
-        <v>0.02434948604075426</v>
+        <v>0.04526352968478164</v>
       </c>
       <c r="D283" t="inlineStr">
         <is>
@@ -79082,13 +79082,13 @@
     </row>
     <row r="284">
       <c r="A284" t="n">
-        <v>52</v>
+        <v>128</v>
       </c>
       <c r="B284" t="n">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="C284" t="n">
-        <v>0.576067092255604</v>
+        <v>0.388861051644304</v>
       </c>
       <c r="D284" t="inlineStr">
         <is>
@@ -79098,13 +79098,13 @@
     </row>
     <row r="285">
       <c r="A285" t="n">
-        <v>121</v>
+        <v>147</v>
       </c>
       <c r="B285" t="n">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="C285" t="n">
-        <v>0.6809437714203316</v>
+        <v>0.63736540965264</v>
       </c>
       <c r="D285" t="inlineStr">
         <is>
@@ -79114,13 +79114,13 @@
     </row>
     <row r="286">
       <c r="A286" t="n">
-        <v>143</v>
+        <v>52</v>
       </c>
       <c r="B286" t="n">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="C286" t="n">
-        <v>0.8563164097165471</v>
+        <v>0.2217610355448335</v>
       </c>
       <c r="D286" t="inlineStr">
         <is>
@@ -79130,13 +79130,13 @@
     </row>
     <row r="287">
       <c r="A287" t="n">
-        <v>48</v>
+        <v>121</v>
       </c>
       <c r="B287" t="n">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="C287" t="n">
-        <v>0.3311174723373911</v>
+        <v>0.552611254738902</v>
       </c>
       <c r="D287" t="inlineStr">
         <is>
@@ -79146,13 +79146,13 @@
     </row>
     <row r="288">
       <c r="A288" t="n">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B288" t="n">
-        <v>155</v>
+        <v>79</v>
       </c>
       <c r="C288" t="n">
-        <v>0.8254231689983109</v>
+        <v>0.7597842201105088</v>
       </c>
       <c r="D288" t="inlineStr">
         <is>
@@ -79162,17 +79162,17 @@
     </row>
     <row r="289">
       <c r="A289" t="n">
-        <v>34</v>
+        <v>146</v>
       </c>
       <c r="B289" t="n">
-        <v>155</v>
+        <v>11</v>
       </c>
       <c r="C289" t="n">
-        <v>0.277261817666144</v>
+        <v>0.1972768451266388</v>
       </c>
       <c r="D289" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>bituminous</t>
         </is>
       </c>
     </row>
@@ -79181,30 +79181,30 @@
         <v>104</v>
       </c>
       <c r="B290" t="n">
-        <v>155</v>
+        <v>11</v>
       </c>
       <c r="C290" t="n">
-        <v>0.6795000401011293</v>
+        <v>0.9361191558388989</v>
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>bituminous</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="n">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="B291" t="n">
-        <v>155</v>
+        <v>11</v>
       </c>
       <c r="C291" t="n">
-        <v>0.605523998127921</v>
+        <v>0.5307255196470104</v>
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>bituminous</t>
         </is>
       </c>
     </row>
@@ -79213,14 +79213,14 @@
         <v>52</v>
       </c>
       <c r="B292" t="n">
-        <v>155</v>
+        <v>11</v>
       </c>
       <c r="C292" t="n">
-        <v>0.1230590248694712</v>
+        <v>0.06681846747859166</v>
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>bituminous</t>
         </is>
       </c>
     </row>
@@ -79229,606 +79229,30 @@
         <v>143</v>
       </c>
       <c r="B293" t="n">
-        <v>155</v>
+        <v>11</v>
       </c>
       <c r="C293" t="n">
-        <v>0.3557956782546093</v>
+        <v>0.3204782694535969</v>
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>bituminous</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="n">
-        <v>146</v>
+        <v>103</v>
       </c>
       <c r="B294" t="n">
-        <v>95</v>
+        <v>143</v>
       </c>
       <c r="C294" t="n">
-        <v>0.3630442223527153</v>
+        <v>0.5239725090670538</v>
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>bituminous</t>
-        </is>
-      </c>
-    </row>
-    <row r="295">
-      <c r="A295" t="n">
-        <v>104</v>
-      </c>
-      <c r="B295" t="n">
-        <v>95</v>
-      </c>
-      <c r="C295" t="n">
-        <v>0.3438084350081263</v>
-      </c>
-      <c r="D295" t="inlineStr">
-        <is>
-          <t>bituminous</t>
-        </is>
-      </c>
-    </row>
-    <row r="296">
-      <c r="A296" t="n">
-        <v>128</v>
-      </c>
-      <c r="B296" t="n">
-        <v>95</v>
-      </c>
-      <c r="C296" t="n">
-        <v>0.3083584297258732</v>
-      </c>
-      <c r="D296" t="inlineStr">
-        <is>
-          <t>bituminous</t>
-        </is>
-      </c>
-    </row>
-    <row r="297">
-      <c r="A297" t="n">
-        <v>52</v>
-      </c>
-      <c r="B297" t="n">
-        <v>95</v>
-      </c>
-      <c r="C297" t="n">
-        <v>0.5218270093478395</v>
-      </c>
-      <c r="D297" t="inlineStr">
-        <is>
-          <t>bituminous</t>
-        </is>
-      </c>
-    </row>
-    <row r="298">
-      <c r="A298" t="n">
-        <v>143</v>
-      </c>
-      <c r="B298" t="n">
-        <v>95</v>
-      </c>
-      <c r="C298" t="n">
-        <v>0.8161391589584358</v>
-      </c>
-      <c r="D298" t="inlineStr">
-        <is>
-          <t>bituminous</t>
-        </is>
-      </c>
-    </row>
-    <row r="299">
-      <c r="A299" t="n">
-        <v>48</v>
-      </c>
-      <c r="B299" t="n">
-        <v>95</v>
-      </c>
-      <c r="C299" t="n">
-        <v>0.1017304640895316</v>
-      </c>
-      <c r="D299" t="inlineStr">
-        <is>
-          <t>bituminous</t>
-        </is>
-      </c>
-    </row>
-    <row r="300">
-      <c r="A300" t="n">
-        <v>146</v>
-      </c>
-      <c r="B300" t="n">
-        <v>152</v>
-      </c>
-      <c r="C300" t="n">
-        <v>0.5871793935809546</v>
-      </c>
-      <c r="D300" t="inlineStr">
-        <is>
           <t>unknown</t>
-        </is>
-      </c>
-    </row>
-    <row r="301">
-      <c r="A301" t="n">
-        <v>34</v>
-      </c>
-      <c r="B301" t="n">
-        <v>152</v>
-      </c>
-      <c r="C301" t="n">
-        <v>0.9537197696640527</v>
-      </c>
-      <c r="D301" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-    </row>
-    <row r="302">
-      <c r="A302" t="n">
-        <v>104</v>
-      </c>
-      <c r="B302" t="n">
-        <v>152</v>
-      </c>
-      <c r="C302" t="n">
-        <v>0.2932872009576085</v>
-      </c>
-      <c r="D302" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-    </row>
-    <row r="303">
-      <c r="A303" t="n">
-        <v>128</v>
-      </c>
-      <c r="B303" t="n">
-        <v>152</v>
-      </c>
-      <c r="C303" t="n">
-        <v>0.1679109584352817</v>
-      </c>
-      <c r="D303" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-    </row>
-    <row r="304">
-      <c r="A304" t="n">
-        <v>147</v>
-      </c>
-      <c r="B304" t="n">
-        <v>152</v>
-      </c>
-      <c r="C304" t="n">
-        <v>0.2270868721159103</v>
-      </c>
-      <c r="D304" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-    </row>
-    <row r="305">
-      <c r="A305" t="n">
-        <v>52</v>
-      </c>
-      <c r="B305" t="n">
-        <v>152</v>
-      </c>
-      <c r="C305" t="n">
-        <v>0.8106316810732421</v>
-      </c>
-      <c r="D305" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-    </row>
-    <row r="306">
-      <c r="A306" t="n">
-        <v>121</v>
-      </c>
-      <c r="B306" t="n">
-        <v>152</v>
-      </c>
-      <c r="C306" t="n">
-        <v>0.3525019553057449</v>
-      </c>
-      <c r="D306" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-    </row>
-    <row r="307">
-      <c r="A307" t="n">
-        <v>143</v>
-      </c>
-      <c r="B307" t="n">
-        <v>152</v>
-      </c>
-      <c r="C307" t="n">
-        <v>0.3615922492106907</v>
-      </c>
-      <c r="D307" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-    </row>
-    <row r="308">
-      <c r="A308" t="n">
-        <v>48</v>
-      </c>
-      <c r="B308" t="n">
-        <v>152</v>
-      </c>
-      <c r="C308" t="n">
-        <v>0.5829350504020845</v>
-      </c>
-      <c r="D308" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-    </row>
-    <row r="309">
-      <c r="A309" t="n">
-        <v>146</v>
-      </c>
-      <c r="B309" t="n">
-        <v>47</v>
-      </c>
-      <c r="C309" t="n">
-        <v>0.2140539599514348</v>
-      </c>
-      <c r="D309" t="inlineStr">
-        <is>
-          <t>bituminous</t>
-        </is>
-      </c>
-    </row>
-    <row r="310">
-      <c r="A310" t="n">
-        <v>34</v>
-      </c>
-      <c r="B310" t="n">
-        <v>47</v>
-      </c>
-      <c r="C310" t="n">
-        <v>0.9420399782472334</v>
-      </c>
-      <c r="D310" t="inlineStr">
-        <is>
-          <t>bituminous</t>
-        </is>
-      </c>
-    </row>
-    <row r="311">
-      <c r="A311" t="n">
-        <v>104</v>
-      </c>
-      <c r="B311" t="n">
-        <v>47</v>
-      </c>
-      <c r="C311" t="n">
-        <v>0.7836556669995561</v>
-      </c>
-      <c r="D311" t="inlineStr">
-        <is>
-          <t>bituminous</t>
-        </is>
-      </c>
-    </row>
-    <row r="312">
-      <c r="A312" t="n">
-        <v>103</v>
-      </c>
-      <c r="B312" t="n">
-        <v>47</v>
-      </c>
-      <c r="C312" t="n">
-        <v>0.2783073982361653</v>
-      </c>
-      <c r="D312" t="inlineStr">
-        <is>
-          <t>bituminous</t>
-        </is>
-      </c>
-    </row>
-    <row r="313">
-      <c r="A313" t="n">
-        <v>52</v>
-      </c>
-      <c r="B313" t="n">
-        <v>47</v>
-      </c>
-      <c r="C313" t="n">
-        <v>0.8405617275947709</v>
-      </c>
-      <c r="D313" t="inlineStr">
-        <is>
-          <t>bituminous</t>
-        </is>
-      </c>
-    </row>
-    <row r="314">
-      <c r="A314" t="n">
-        <v>143</v>
-      </c>
-      <c r="B314" t="n">
-        <v>47</v>
-      </c>
-      <c r="C314" t="n">
-        <v>0.1707706149181917</v>
-      </c>
-      <c r="D314" t="inlineStr">
-        <is>
-          <t>bituminous</t>
-        </is>
-      </c>
-    </row>
-    <row r="315">
-      <c r="A315" t="n">
-        <v>146</v>
-      </c>
-      <c r="B315" t="n">
-        <v>79</v>
-      </c>
-      <c r="C315" t="n">
-        <v>0.1848310823857744</v>
-      </c>
-      <c r="D315" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-    </row>
-    <row r="316">
-      <c r="A316" t="n">
-        <v>34</v>
-      </c>
-      <c r="B316" t="n">
-        <v>79</v>
-      </c>
-      <c r="C316" t="n">
-        <v>0.6954228604764011</v>
-      </c>
-      <c r="D316" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-    </row>
-    <row r="317">
-      <c r="A317" t="n">
-        <v>104</v>
-      </c>
-      <c r="B317" t="n">
-        <v>79</v>
-      </c>
-      <c r="C317" t="n">
-        <v>0.2474311993863385</v>
-      </c>
-      <c r="D317" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-    </row>
-    <row r="318">
-      <c r="A318" t="n">
-        <v>128</v>
-      </c>
-      <c r="B318" t="n">
-        <v>79</v>
-      </c>
-      <c r="C318" t="n">
-        <v>0.6387385628136152</v>
-      </c>
-      <c r="D318" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-    </row>
-    <row r="319">
-      <c r="A319" t="n">
-        <v>147</v>
-      </c>
-      <c r="B319" t="n">
-        <v>79</v>
-      </c>
-      <c r="C319" t="n">
-        <v>0.2012959210918128</v>
-      </c>
-      <c r="D319" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-    </row>
-    <row r="320">
-      <c r="A320" t="n">
-        <v>52</v>
-      </c>
-      <c r="B320" t="n">
-        <v>79</v>
-      </c>
-      <c r="C320" t="n">
-        <v>0.5066587992308162</v>
-      </c>
-      <c r="D320" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-    </row>
-    <row r="321">
-      <c r="A321" t="n">
-        <v>121</v>
-      </c>
-      <c r="B321" t="n">
-        <v>79</v>
-      </c>
-      <c r="C321" t="n">
-        <v>0.8713234364149867</v>
-      </c>
-      <c r="D321" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-    </row>
-    <row r="322">
-      <c r="A322" t="n">
-        <v>143</v>
-      </c>
-      <c r="B322" t="n">
-        <v>79</v>
-      </c>
-      <c r="C322" t="n">
-        <v>0.5662103792068846</v>
-      </c>
-      <c r="D322" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-    </row>
-    <row r="323">
-      <c r="A323" t="n">
-        <v>146</v>
-      </c>
-      <c r="B323" t="n">
-        <v>11</v>
-      </c>
-      <c r="C323" t="n">
-        <v>0.30685019073779</v>
-      </c>
-      <c r="D323" t="inlineStr">
-        <is>
-          <t>bituminous</t>
-        </is>
-      </c>
-    </row>
-    <row r="324">
-      <c r="A324" t="n">
-        <v>104</v>
-      </c>
-      <c r="B324" t="n">
-        <v>11</v>
-      </c>
-      <c r="C324" t="n">
-        <v>0.4115160785830871</v>
-      </c>
-      <c r="D324" t="inlineStr">
-        <is>
-          <t>bituminous</t>
-        </is>
-      </c>
-    </row>
-    <row r="325">
-      <c r="A325" t="n">
-        <v>128</v>
-      </c>
-      <c r="B325" t="n">
-        <v>11</v>
-      </c>
-      <c r="C325" t="n">
-        <v>0.3565413089325663</v>
-      </c>
-      <c r="D325" t="inlineStr">
-        <is>
-          <t>bituminous</t>
-        </is>
-      </c>
-    </row>
-    <row r="326">
-      <c r="A326" t="n">
-        <v>147</v>
-      </c>
-      <c r="B326" t="n">
-        <v>11</v>
-      </c>
-      <c r="C326" t="n">
-        <v>0.5405019709978334</v>
-      </c>
-      <c r="D326" t="inlineStr">
-        <is>
-          <t>bituminous</t>
-        </is>
-      </c>
-    </row>
-    <row r="327">
-      <c r="A327" t="n">
-        <v>52</v>
-      </c>
-      <c r="B327" t="n">
-        <v>11</v>
-      </c>
-      <c r="C327" t="n">
-        <v>0.5051033112755541</v>
-      </c>
-      <c r="D327" t="inlineStr">
-        <is>
-          <t>bituminous</t>
-        </is>
-      </c>
-    </row>
-    <row r="328">
-      <c r="A328" t="n">
-        <v>121</v>
-      </c>
-      <c r="B328" t="n">
-        <v>11</v>
-      </c>
-      <c r="C328" t="n">
-        <v>0.7314024284289271</v>
-      </c>
-      <c r="D328" t="inlineStr">
-        <is>
-          <t>bituminous</t>
-        </is>
-      </c>
-    </row>
-    <row r="329">
-      <c r="A329" t="n">
-        <v>143</v>
-      </c>
-      <c r="B329" t="n">
-        <v>11</v>
-      </c>
-      <c r="C329" t="n">
-        <v>0.2406412425751817</v>
-      </c>
-      <c r="D329" t="inlineStr">
-        <is>
-          <t>bituminous</t>
-        </is>
-      </c>
-    </row>
-    <row r="330">
-      <c r="A330" t="n">
-        <v>48</v>
-      </c>
-      <c r="B330" t="n">
-        <v>11</v>
-      </c>
-      <c r="C330" t="n">
-        <v>0.177019027043647</v>
-      </c>
-      <c r="D330" t="inlineStr">
-        <is>
-          <t>bituminous</t>
         </is>
       </c>
     </row>

</xml_diff>